<commit_message>
Add - Extent Report  - base level
Add - Data Excel  - base level
</commit_message>
<xml_diff>
--- a/testdata/BillingCenter.xlsx
+++ b/testdata/BillingCenter.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\asrikanth\eclipse-workspace\GWFW_CMPCBCCC\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519EC6DF-31C8-46D7-B88E-FF1745A48A80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9BF5CA-B910-40B1-B5D7-345864264D57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27840" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27840" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Account" sheetId="2" r:id="rId2"/>
     <sheet name="Policy" sheetId="3" r:id="rId3"/>
-    <sheet name="Invoice" sheetId="4" r:id="rId4"/>
+    <sheet name="AcctSummary" sheetId="5" r:id="rId4"/>
+    <sheet name="Invoice" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,14 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>TD_UserName</t>
   </si>
   <si>
-    <t>TD_Passwprd</t>
-  </si>
-  <si>
     <t>su</t>
   </si>
   <si>
@@ -106,12 +104,129 @@
   </si>
   <si>
     <t>User7</t>
+  </si>
+  <si>
+    <t>TD_Password</t>
+  </si>
+  <si>
+    <t>TD_AccountName</t>
+  </si>
+  <si>
+    <t>TD_AccountType</t>
+  </si>
+  <si>
+    <t>TD_BillingPlan</t>
+  </si>
+  <si>
+    <t>TD_DelinquencyPlan</t>
+  </si>
+  <si>
+    <t>TD_SendInvoicesBy</t>
+  </si>
+  <si>
+    <t>TD_CompanyName</t>
+  </si>
+  <si>
+    <t>QA1BILLINGPLAN01</t>
+  </si>
+  <si>
+    <t>BillPlan1</t>
+  </si>
+  <si>
+    <t>BillPlan2</t>
+  </si>
+  <si>
+    <t>BillPlan3</t>
+  </si>
+  <si>
+    <t>BillPlan4</t>
+  </si>
+  <si>
+    <t>BillPlan5</t>
+  </si>
+  <si>
+    <t>Insured</t>
+  </si>
+  <si>
+    <t>Equity-Based Delinquency Plan</t>
+  </si>
+  <si>
+    <t>Wright Construction</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Automation10</t>
+  </si>
+  <si>
+    <t>Direct Bill</t>
+  </si>
+  <si>
+    <t>TD_BillingMethod</t>
+  </si>
+  <si>
+    <t>TD_PaymentPlan</t>
+  </si>
+  <si>
+    <t>B Monthly 10% Down, Max 11 installments</t>
+  </si>
+  <si>
+    <t>PaymentPlan1</t>
+  </si>
+  <si>
+    <t>PaymentPlan2</t>
+  </si>
+  <si>
+    <t>PaymentPlan3</t>
+  </si>
+  <si>
+    <t>PaymentPlan4</t>
+  </si>
+  <si>
+    <t>PaymentPlan5</t>
+  </si>
+  <si>
+    <t>TD_PayoffAmount</t>
+  </si>
+  <si>
+    <t>TD_PolicyNumber</t>
+  </si>
+  <si>
+    <t>TD_TotalValue</t>
+  </si>
+  <si>
+    <t>AccountSummary1</t>
+  </si>
+  <si>
+    <t>AccountSummary2</t>
+  </si>
+  <si>
+    <t>AccountSummary3</t>
+  </si>
+  <si>
+    <t>AccountSummary4</t>
+  </si>
+  <si>
+    <t>AccountSummary5</t>
+  </si>
+  <si>
+    <t>TD_ChargesType</t>
+  </si>
+  <si>
+    <t>TD_ChargesAmount</t>
+  </si>
+  <si>
+    <t>Premium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -184,6 +299,26 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,101 +615,101 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -585,29 +720,314 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3520C8-D792-4977-99E0-C45876A8E20A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B240F2F-8AD3-49E3-9150-9222387F22C2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6705243-A037-4CA9-B29E-68E745D48062}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="11">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729A753F-FC84-49D2-8EB2-5A2921F6B535}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
reporting folder structure updated
</commit_message>
<xml_diff>
--- a/testdata/BillingCenter.xlsx
+++ b/testdata/BillingCenter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labor\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labor\git\blackcomb\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD8B2D9-EEAD-4FC4-9D9D-AFCF97F1EE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0F308E-2688-45B8-A804-85BB486126EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -1343,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609C42BF-E54F-4C6E-8490-1C1A1918364C}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="E2" s="34">
         <f t="shared" ref="E2:E3" ca="1" si="0">TODAY()</f>
-        <v>44345</v>
+        <v>44350</v>
       </c>
       <c r="F2" s="46" t="s">
         <v>128</v>
@@ -1462,7 +1462,7 @@
       <c r="D3" s="29"/>
       <c r="E3" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>44345</v>
+        <v>44350</v>
       </c>
       <c r="F3" s="29" t="s">
         <v>39</v>
@@ -1762,7 +1762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03A182C-4A83-40EC-82BA-4154075170BB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="E2" s="44">
         <f ca="1">searchValues!E3</f>
-        <v>44345</v>
+        <v>44350</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>37</v>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="C2" s="50">
         <f ca="1">searchValues!E3</f>
-        <v>44345</v>
+        <v>44350</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Billing Center and Claim center Added
</commit_message>
<xml_diff>
--- a/testdata/BillingCenter.xlsx
+++ b/testdata/BillingCenter.xlsx
@@ -1,41 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akash Gowda\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC1\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3301A4F3-814B-4B44-B25E-07F28F5CBD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35E499F-651E-4350-AD73-2C60B3D22CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19680" windowHeight="11760" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="searchValues" sheetId="10" r:id="rId2"/>
-    <sheet name="Account" sheetId="2" r:id="rId3"/>
-    <sheet name="Policy" sheetId="3" r:id="rId4"/>
-    <sheet name="DirectBillPayment" sheetId="11" r:id="rId5"/>
-    <sheet name="AcctSummary" sheetId="5" r:id="rId6"/>
-    <sheet name="AcctDetails" sheetId="6" r:id="rId7"/>
-    <sheet name="Contacts" sheetId="7" r:id="rId8"/>
-    <sheet name="Invoices" sheetId="4" r:id="rId9"/>
-    <sheet name="PolicySummary" sheetId="8" r:id="rId10"/>
-    <sheet name="PolicyDetails" sheetId="9" r:id="rId11"/>
+    <sheet name="npInvoices" sheetId="13" r:id="rId3"/>
+    <sheet name="payment" sheetId="15" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="14" r:id="rId5"/>
+    <sheet name="Account" sheetId="2" r:id="rId6"/>
+    <sheet name="Policy" sheetId="3" r:id="rId7"/>
+    <sheet name="DirectBillPayment" sheetId="11" r:id="rId8"/>
+    <sheet name="AcctSummary" sheetId="5" r:id="rId9"/>
+    <sheet name="Disbursement" sheetId="12" r:id="rId10"/>
+    <sheet name="AcctDetails" sheetId="6" r:id="rId11"/>
+    <sheet name="Contacts" sheetId="7" r:id="rId12"/>
+    <sheet name="Invoices" sheetId="4" r:id="rId13"/>
+    <sheet name="PolicySummary" sheetId="8" r:id="rId14"/>
+    <sheet name="PolicyDetails" sheetId="9" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="167">
   <si>
     <t>su</t>
   </si>
@@ -454,15 +465,102 @@
   </si>
   <si>
     <t>Billed</t>
+  </si>
+  <si>
+    <t>TD_Unapplied</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>UnappliedFund</t>
+  </si>
+  <si>
+    <t>PaymentDate</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>DisbursementStatus1</t>
+  </si>
+  <si>
+    <t>DisbursementStatus2</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>Sent</t>
+  </si>
+  <si>
+    <t>AUT_Disbursement_Manual</t>
+  </si>
+  <si>
+    <t>AUT_Disbursement_Automatic</t>
+  </si>
+  <si>
+    <t>Nick Automation</t>
+  </si>
+  <si>
+    <t>AUT_NonPayment_Delequency</t>
+  </si>
+  <si>
+    <t>Commercial Auto</t>
+  </si>
+  <si>
+    <t>sds bc</t>
+  </si>
+  <si>
+    <t>AUT_BC_Payment</t>
+  </si>
+  <si>
+    <t>NP_InvoiceStream</t>
+  </si>
+  <si>
+    <t>NP_Invoice_BillDate</t>
+  </si>
+  <si>
+    <t>NP_Invoice_DueDate</t>
+  </si>
+  <si>
+    <t>NP_Status</t>
+  </si>
+  <si>
+    <t>InvoicesStream_DefaultDayofMonth</t>
+  </si>
+  <si>
+    <t>InvoicesStream_InvoiceDays</t>
+  </si>
+  <si>
+    <t>InvoicesStream_Default</t>
+  </si>
+  <si>
+    <t>3651040130 (Monthly)</t>
+  </si>
+  <si>
+    <t>PaymentInstrument</t>
+  </si>
+  <si>
+    <t>Cash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
+  <numFmts count="5">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="mm\/dd\/yyyy"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="167" formatCode="dd\/mm\/yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -566,7 +664,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -600,11 +698,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -679,7 +799,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -705,7 +825,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -721,11 +841,11 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -738,6 +858,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,9 +1165,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1200,6 +1349,46 @@
         <v>63</v>
       </c>
     </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="66" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1207,6 +1396,396 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6623F5E3-B6AD-4B62-877A-4DCEFEC224B3}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2">
+        <f>searchValues!$G$5</f>
+        <v>2058887593</v>
+      </c>
+      <c r="C2" t="str">
+        <f>searchValues!$F$4</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="64">
+        <v>100</v>
+      </c>
+      <c r="F2" s="65">
+        <f ca="1">TODAY()</f>
+        <v>44487</v>
+      </c>
+      <c r="G2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3">
+        <f>searchValues!$G$5</f>
+        <v>2058887593</v>
+      </c>
+      <c r="C3" t="str">
+        <f>searchValues!$F$4</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="F3" s="65">
+        <f ca="1">TODAY()</f>
+        <v>44487</v>
+      </c>
+      <c r="H3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C58BF8B-1280-4F12-9EAD-0C522762E5C1}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="32" t="str">
+        <f>searchValues!F3</f>
+        <v>DgljZjCqj Automation</v>
+      </c>
+      <c r="C2" s="33" t="str">
+        <f>searchValues!G3</f>
+        <v>0328737272</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="44">
+        <f ca="1">searchValues!E3</f>
+        <v>44487</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="31"/>
+      <c r="J2" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BA4B8D-994F-445A-8329-A78DC1606E04}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="str">
+        <f>searchValues!F3</f>
+        <v>DgljZjCqj Automation</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" t="str">
+        <f>searchValues!M3</f>
+        <v>Alaska</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3">
+        <f>searchValues!M4</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729A753F-FC84-49D2-8EB2-5A2921F6B535}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="50">
+        <f ca="1">searchValues!E3</f>
+        <v>44487</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71F8AC9-A36C-49D9-9891-077F11566646}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1277,7 +1856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222CFAE0-9168-4C02-A943-4F9BE574003A}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1362,10 +1941,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609C42BF-E54F-4C6E-8490-1C1A1918364C}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,7 +2018,7 @@
       </c>
       <c r="E2" s="34">
         <f t="shared" ref="E2:E3" ca="1" si="0">TODAY()</f>
-        <v>44354</v>
+        <v>44487</v>
       </c>
       <c r="F2" s="46" t="s">
         <v>124</v>
@@ -1483,7 +2062,7 @@
       <c r="D3" s="29"/>
       <c r="E3" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>44354</v>
+        <v>44487</v>
       </c>
       <c r="F3" s="54" t="s">
         <v>132</v>
@@ -1504,6 +2083,167 @@
       </c>
       <c r="M3" s="36" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="26">
+        <v>2058887593</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="68" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="26">
+        <v>2058887593</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" s="20">
+        <v>1580543906</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="M6" s="36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="20">
+        <v>1580543906</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1624AA-EFC2-4B9A-B805-8486152D6359}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="69">
+        <v>44387</v>
+      </c>
+      <c r="D2" s="69">
+        <v>44207</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="69">
+        <v>44387</v>
+      </c>
+      <c r="D3" s="69">
+        <v>44207</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1511,7 +2251,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59830DF0-FAD5-472D-8467-4240A14AC5A6}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3651C9-5051-4CB9-9FEB-B72D129372D3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3520C8-D792-4977-99E0-C45876A8E20A}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -1663,7 +2456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B240F2F-8AD3-49E3-9150-9222387F22C2}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -1779,12 +2572,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03A182C-4A83-40EC-82BA-4154075170BB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,28 +2608,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6705243-A037-4CA9-B29E-68E745D48062}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="8"/>
+    <col min="9" max="9" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
@@ -1861,8 +2654,11 @@
       <c r="H1" s="18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>111</v>
       </c>
@@ -1888,7 +2684,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>53</v>
       </c>
@@ -1900,7 +2696,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>54</v>
       </c>
@@ -1912,7 +2708,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>55</v>
       </c>
@@ -1924,297 +2720,67 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C58BF8B-1280-4F12-9EAD-0C522762E5C1}">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="24"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="32" t="str">
-        <f>searchValues!F3</f>
-        <v>DgljZjCqj Automation</v>
-      </c>
-      <c r="C2" s="33" t="str">
-        <f>searchValues!G3</f>
-        <v>0328737272</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="44">
-        <f ca="1">searchValues!E3</f>
-        <v>44354</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BA4B8D-994F-445A-8329-A78DC1606E04}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" t="str">
-        <f>searchValues!F3</f>
-        <v>DgljZjCqj Automation</v>
-      </c>
-      <c r="D2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E2" s="56" t="s">
-        <v>136</v>
-      </c>
-      <c r="G2" t="str">
-        <f>searchValues!M3</f>
-        <v>Alaska</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3">
-        <f>searchValues!M4</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729A753F-FC84-49D2-8EB2-5A2921F6B535}">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="50">
-        <f ca="1">searchValues!E3</f>
-        <v>44354</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+    </row>
+    <row r="7" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="61" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="8" t="str">
+        <f>searchValues!$F$5</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>searchValues!$F$5</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="67">
+        <v>3499</v>
+      </c>
+      <c r="H7" s="67">
+        <v>3499</v>
+      </c>
+      <c r="I7" s="63">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="66" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="8" t="str">
+        <f>searchValues!$F$5</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="C8" s="8" t="str">
+        <f>searchValues!$F$5</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="67">
+        <v>3499</v>
+      </c>
+      <c r="H8" s="67">
+        <v>3499</v>
+      </c>
+      <c r="I8" s="63">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
PersonalAuto and BC scripts updated(Demo)
</commit_message>
<xml_diff>
--- a/testdata/BillingCenter.xlsx
+++ b/testdata/BillingCenter.xlsx
@@ -1,33 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\agowda\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35E499F-651E-4350-AD73-2C60B3D22CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94A2503-F685-4654-A40B-8FC4C1A500F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19680" windowHeight="10320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="searchValues" sheetId="10" r:id="rId2"/>
     <sheet name="npInvoices" sheetId="13" r:id="rId3"/>
     <sheet name="payment" sheetId="15" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="14" r:id="rId5"/>
-    <sheet name="Account" sheetId="2" r:id="rId6"/>
-    <sheet name="Policy" sheetId="3" r:id="rId7"/>
-    <sheet name="DirectBillPayment" sheetId="11" r:id="rId8"/>
-    <sheet name="AcctSummary" sheetId="5" r:id="rId9"/>
-    <sheet name="Disbursement" sheetId="12" r:id="rId10"/>
-    <sheet name="AcctDetails" sheetId="6" r:id="rId11"/>
-    <sheet name="Contacts" sheetId="7" r:id="rId12"/>
-    <sheet name="Invoices" sheetId="4" r:id="rId13"/>
-    <sheet name="PolicySummary" sheetId="8" r:id="rId14"/>
-    <sheet name="PolicyDetails" sheetId="9" r:id="rId15"/>
+    <sheet name="Account" sheetId="2" r:id="rId5"/>
+    <sheet name="Policy" sheetId="3" r:id="rId6"/>
+    <sheet name="DirectBillPayment" sheetId="11" r:id="rId7"/>
+    <sheet name="AcctSummary" sheetId="5" r:id="rId8"/>
+    <sheet name="Disbursement" sheetId="12" r:id="rId9"/>
+    <sheet name="AcctDetails" sheetId="6" r:id="rId10"/>
+    <sheet name="Contacts" sheetId="7" r:id="rId11"/>
+    <sheet name="Invoices" sheetId="4" r:id="rId12"/>
+    <sheet name="PolicySummary" sheetId="8" r:id="rId13"/>
+    <sheet name="PolicyDetails" sheetId="9" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -441,15 +442,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>8233431666-1</t>
-  </si>
-  <si>
-    <t>DgljZjCqj Automation</t>
-  </si>
-  <si>
-    <t>0328737272</t>
-  </si>
-  <si>
     <t>AUT_PA_BC_Invoice_02</t>
   </si>
   <si>
@@ -549,6 +541,15 @@
   </si>
   <si>
     <t>Cash</t>
+  </si>
+  <si>
+    <t>0266579499</t>
+  </si>
+  <si>
+    <t>0266579499-1</t>
+  </si>
+  <si>
+    <t>GZQtMQMuM Automation</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1352,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>0</v>
@@ -1371,7 +1372,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>0</v>
@@ -1396,121 +1397,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6623F5E3-B6AD-4B62-877A-4DCEFEC224B3}">
-  <dimension ref="A1:K3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2">
-        <f>searchValues!$G$5</f>
-        <v>2058887593</v>
-      </c>
-      <c r="C2" t="str">
-        <f>searchValues!$F$4</f>
-        <v>Nick Automation</v>
-      </c>
-      <c r="D2" s="64" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" s="64">
-        <v>100</v>
-      </c>
-      <c r="F2" s="65">
-        <f ca="1">TODAY()</f>
-        <v>44487</v>
-      </c>
-      <c r="G2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H2" t="s">
-        <v>148</v>
-      </c>
-      <c r="I2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3">
-        <f>searchValues!$G$5</f>
-        <v>2058887593</v>
-      </c>
-      <c r="C3" t="str">
-        <f>searchValues!$F$4</f>
-        <v>Nick Automation</v>
-      </c>
-      <c r="F3" s="65">
-        <f ca="1">TODAY()</f>
-        <v>44487</v>
-      </c>
-      <c r="H3" t="s">
-        <v>148</v>
-      </c>
-      <c r="I3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C58BF8B-1280-4F12-9EAD-0C522762E5C1}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,18 +1461,18 @@
       </c>
       <c r="B2" s="32" t="str">
         <f>searchValues!F3</f>
-        <v>DgljZjCqj Automation</v>
-      </c>
-      <c r="C2" s="33" t="str">
+        <v>GZQtMQMuM Automation</v>
+      </c>
+      <c r="C2" s="33">
         <f>searchValues!G3</f>
-        <v>0328737272</v>
+        <v>3195635219</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>35</v>
       </c>
       <c r="E2" s="44">
         <f ca="1">searchValues!E3</f>
-        <v>44487</v>
+        <v>44578</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>37</v>
@@ -1606,7 +1497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BA4B8D-994F-445A-8329-A78DC1606E04}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1652,17 +1543,17 @@
         <v>111</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C2" t="str">
         <f>searchValues!F3</f>
-        <v>DgljZjCqj Automation</v>
+        <v>GZQtMQMuM Automation</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G2" t="str">
         <f>searchValues!M3</f>
@@ -1671,7 +1562,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>81</v>
@@ -1695,7 +1586,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729A753F-FC84-49D2-8EB2-5A2921F6B535}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1754,7 +1645,7 @@
       </c>
       <c r="C2" s="50">
         <f ca="1">searchValues!E3</f>
-        <v>44487</v>
+        <v>44578</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>90</v>
@@ -1766,7 +1657,7 @@
         <v>92</v>
       </c>
       <c r="G2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H2" t="s">
         <v>92</v>
@@ -1785,7 +1676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71F8AC9-A36C-49D9-9891-077F11566646}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1856,7 +1747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222CFAE0-9168-4C02-A943-4F9BE574003A}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1909,7 +1800,7 @@
       </c>
       <c r="B2" t="str">
         <f>searchValues!J3</f>
-        <v>8233431666-1</v>
+        <v>0266579499-1</v>
       </c>
       <c r="C2" t="s">
         <v>94</v>
@@ -1943,8 +1834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609C42BF-E54F-4C6E-8490-1C1A1918364C}">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2018,7 +1909,7 @@
       </c>
       <c r="E2" s="34">
         <f t="shared" ref="E2:E3" ca="1" si="0">TODAY()</f>
-        <v>44487</v>
+        <v>44578</v>
       </c>
       <c r="F2" s="46" t="s">
         <v>124</v>
@@ -2062,20 +1953,22 @@
       <c r="D3" s="29"/>
       <c r="E3" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>44487</v>
+        <v>44578</v>
       </c>
       <c r="F3" s="54" t="s">
-        <v>132</v>
-      </c>
-      <c r="G3" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29">
-        <v>8233431666</v>
-      </c>
-      <c r="J3" s="29" t="s">
-        <v>131</v>
+        <v>166</v>
+      </c>
+      <c r="G3" s="55">
+        <v>3195635219</v>
+      </c>
+      <c r="H3" s="29">
+        <v>608519016</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>165</v>
       </c>
       <c r="K3" s="29"/>
       <c r="L3" s="35" t="s">
@@ -2087,10 +1980,10 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G4" s="26">
         <v>2058887593</v>
@@ -2098,10 +1991,10 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G5" s="26">
         <v>2058887593</v>
@@ -2109,13 +2002,13 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F6" s="54" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G6" s="20">
         <v>1580543906</v>
@@ -2129,10 +2022,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F7" s="54" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G7" s="20">
         <v>1580543906</v>
@@ -2158,7 +2051,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2173,33 +2066,33 @@
         <v>2</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>160</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C2" s="69">
         <v>44387</v>
@@ -2208,7 +2101,7 @@
         <v>44207</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F2">
         <v>15</v>
@@ -2222,10 +2115,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C3" s="69">
         <v>44387</v>
@@ -2234,7 +2127,7 @@
         <v>44207</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F3">
         <v>15</v>
@@ -2255,7 +2148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59830DF0-FAD5-472D-8467-4240A14AC5A6}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -2273,18 +2166,18 @@
         <v>120</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B2">
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2293,23 +2186,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3651C9-5051-4CB9-9FEB-B72D129372D3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3520C8-D792-4977-99E0-C45876A8E20A}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2365,11 +2246,11 @@
       </c>
       <c r="B2" s="29" t="str">
         <f>searchValues!F3</f>
-        <v>DgljZjCqj Automation</v>
-      </c>
-      <c r="C2" s="28" t="str">
+        <v>GZQtMQMuM Automation</v>
+      </c>
+      <c r="C2" s="28">
         <f>searchValues!G3</f>
-        <v>0328737272</v>
+        <v>3195635219</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>66</v>
@@ -2456,12 +2337,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B240F2F-8AD3-49E3-9150-9222387F22C2}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2502,9 +2383,9 @@
       <c r="A2" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2" s="41" t="str">
         <f>searchValues!I3</f>
-        <v>8233431666</v>
+        <v>0266579499</v>
       </c>
       <c r="C2" s="42" t="s">
         <v>39</v>
@@ -2572,7 +2453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03A182C-4A83-40EC-82BA-4154075170BB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2608,12 +2489,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6705243-A037-4CA9-B29E-68E745D48062}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,7 +2536,7 @@
         <v>49</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2664,14 +2545,14 @@
       </c>
       <c r="B2" s="7" t="str">
         <f>searchValues!F3</f>
-        <v>DgljZjCqj Automation</v>
+        <v>GZQtMQMuM Automation</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>searchValues!F3</f>
-        <v>DgljZjCqj Automation</v>
+        <v>GZQtMQMuM Automation</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>71</v>
@@ -2734,7 +2615,7 @@
     </row>
     <row r="7" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="61" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B7" s="8" t="str">
         <f>searchValues!$F$5</f>
@@ -2759,7 +2640,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="66" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B8" s="8" t="str">
         <f>searchValues!$F$5</f>
@@ -2787,4 +2668,114 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6623F5E3-B6AD-4B62-877A-4DCEFEC224B3}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2">
+        <f>searchValues!$G$5</f>
+        <v>2058887593</v>
+      </c>
+      <c r="C2" t="str">
+        <f>searchValues!$F$4</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="64">
+        <v>100</v>
+      </c>
+      <c r="F2" s="65">
+        <f ca="1">TODAY()</f>
+        <v>44578</v>
+      </c>
+      <c r="G2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3">
+        <f>searchValues!$G$5</f>
+        <v>2058887593</v>
+      </c>
+      <c r="C3" t="str">
+        <f>searchValues!$F$4</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="F3" s="65">
+        <f ca="1">TODAY()</f>
+        <v>44578</v>
+      </c>
+      <c r="H3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
PC- CA, BO ; BC- Updated
</commit_message>
<xml_diff>
--- a/testdata/BillingCenter.xlsx
+++ b/testdata/BillingCenter.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\agowda\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIG\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94A2503-F685-4654-A40B-8FC4C1A500F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D50062-C8C5-418A-9F2E-985CF586C6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19680" windowHeight="10320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="searchValues" sheetId="10" r:id="rId2"/>
     <sheet name="npInvoices" sheetId="13" r:id="rId3"/>
     <sheet name="payment" sheetId="15" r:id="rId4"/>
-    <sheet name="Account" sheetId="2" r:id="rId5"/>
-    <sheet name="Policy" sheetId="3" r:id="rId6"/>
-    <sheet name="DirectBillPayment" sheetId="11" r:id="rId7"/>
-    <sheet name="AcctSummary" sheetId="5" r:id="rId8"/>
-    <sheet name="Disbursement" sheetId="12" r:id="rId9"/>
-    <sheet name="AcctDetails" sheetId="6" r:id="rId10"/>
-    <sheet name="Contacts" sheetId="7" r:id="rId11"/>
-    <sheet name="Invoices" sheetId="4" r:id="rId12"/>
-    <sheet name="PolicySummary" sheetId="8" r:id="rId13"/>
-    <sheet name="PolicyDetails" sheetId="9" r:id="rId14"/>
+    <sheet name="TroubleTicket" sheetId="16" r:id="rId5"/>
+    <sheet name="Account" sheetId="2" r:id="rId6"/>
+    <sheet name="Policy" sheetId="3" r:id="rId7"/>
+    <sheet name="DirectBillPayment" sheetId="11" r:id="rId8"/>
+    <sheet name="AcctSummary" sheetId="5" r:id="rId9"/>
+    <sheet name="Disbursement" sheetId="12" r:id="rId10"/>
+    <sheet name="AcctDetails" sheetId="6" r:id="rId11"/>
+    <sheet name="Contacts" sheetId="7" r:id="rId12"/>
+    <sheet name="Invoices" sheetId="4" r:id="rId13"/>
+    <sheet name="PolicySummary" sheetId="8" r:id="rId14"/>
+    <sheet name="PolicyDetails" sheetId="9" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="192">
   <si>
     <t>su</t>
   </si>
@@ -550,6 +551,81 @@
   </si>
   <si>
     <t>GZQtMQMuM Automation</t>
+  </si>
+  <si>
+    <t>BC_Disbursement_Manual</t>
+  </si>
+  <si>
+    <t>TroubleTickets</t>
+  </si>
+  <si>
+    <t>aapplegate</t>
+  </si>
+  <si>
+    <t>SuspensePaymentProcess</t>
+  </si>
+  <si>
+    <t>PaymentSchedule</t>
+  </si>
+  <si>
+    <t>ReversePayment</t>
+  </si>
+  <si>
+    <t>GTTestingWCm</t>
+  </si>
+  <si>
+    <t>8575352547-1</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>ReleaseDate</t>
+  </si>
+  <si>
+    <t>Disaster Hold</t>
+  </si>
+  <si>
+    <t>Urgent</t>
+  </si>
+  <si>
+    <t>03/31/2022</t>
+  </si>
+  <si>
+    <t>Pending Cancellation</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>A Monthly 10% Down, 9 Max installments</t>
+  </si>
+  <si>
+    <t>TD_NewPaymentPlan</t>
+  </si>
+  <si>
+    <t>09/25/2022</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>ReverseFee</t>
+  </si>
+  <si>
+    <t>Reversal_Reason</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>Payment Declined</t>
   </si>
 </sst>
 </file>
@@ -557,13 +633,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="mm\/dd\/yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="167" formatCode="dd\/mm\/yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,6 +671,21 @@
       <color rgb="FF1F1F1F"/>
       <name val="Source Sans Pro"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -665,7 +756,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -699,73 +790,27 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -787,9 +832,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -800,21 +842,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -827,6 +854,85 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -842,50 +948,88 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1166,227 +1310,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.85546875" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" s="43" customFormat="1">
+      <c r="A1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="41" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="41" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="66" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="85" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="85" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1397,6 +1622,147 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6623F5E3-B6AD-4B62-877A-4DCEFEC224B3}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2">
+        <f>searchValues!$G$5</f>
+        <v>2058887593</v>
+      </c>
+      <c r="C2" t="str">
+        <f>searchValues!$F$4</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="34">
+        <v>100</v>
+      </c>
+      <c r="F2" s="35">
+        <f ca="1">TODAY()</f>
+        <v>44657</v>
+      </c>
+      <c r="G2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3">
+        <f>searchValues!$G$5</f>
+        <v>2058887593</v>
+      </c>
+      <c r="C3" t="str">
+        <f>searchValues!$F$4</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="F3" s="35">
+        <f ca="1">TODAY()</f>
+        <v>44657</v>
+      </c>
+      <c r="H3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4">
+        <f>searchValues!$G$5</f>
+        <v>2058887593</v>
+      </c>
+      <c r="C4" t="str">
+        <f>searchValues!$F$4</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C58BF8B-1280-4F12-9EAD-0C522762E5C1}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1404,90 +1770,90 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="22.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:11" s="9" customFormat="1">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:11">
+      <c r="A2" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="32" t="str">
+      <c r="B2" s="21" t="str">
         <f>searchValues!F3</f>
         <v>GZQtMQMuM Automation</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="22">
         <f>searchValues!G3</f>
         <v>3195635219</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="44">
+      <c r="E2" s="28">
         <f ca="1">searchValues!E3</f>
-        <v>44578</v>
-      </c>
-      <c r="F2" s="31" t="s">
+        <v>44657</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="18" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1497,7 +1863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BA4B8D-994F-445A-8329-A78DC1606E04}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1505,7 +1871,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -1515,34 +1881,34 @@
     <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="75">
       <c r="A2" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="10" t="s">
         <v>132</v>
       </c>
       <c r="C2" t="str">
@@ -1552,7 +1918,7 @@
       <c r="D2" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="32" t="s">
         <v>133</v>
       </c>
       <c r="G2" t="str">
@@ -1560,11 +1926,11 @@
         <v>Alaska</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="10" t="s">
         <v>81</v>
       </c>
       <c r="C3" t="s">
@@ -1586,7 +1952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729A753F-FC84-49D2-8EB2-5A2921F6B535}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1594,7 +1960,7 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -1607,50 +1973,50 @@
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="50">
+      <c r="C2" s="29">
         <f ca="1">searchValues!E3</f>
-        <v>44578</v>
-      </c>
-      <c r="D2" s="21" t="s">
+        <v>44657</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="11" t="s">
         <v>94</v>
       </c>
       <c r="F2" t="s">
@@ -1666,8 +2032,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+    <row r="3" spans="1:9">
+      <c r="A3" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1676,15 +2042,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71F8AC9-A36C-49D9-9891-077F11566646}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
@@ -1693,32 +2059,37 @@
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="98" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="98"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -1739,6 +2110,32 @@
       </c>
       <c r="G2" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="97" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="96" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="96" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="96" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="96" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="96" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1747,13 +2144,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222CFAE0-9168-4C02-A943-4F9BE574003A}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
@@ -1765,36 +2162,36 @@
     <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -1832,213 +2229,337 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609C42BF-E54F-4C6E-8490-1C1A1918364C}">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="47.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="22.28515625" style="26"/>
+    <col min="1" max="1" width="47.140625" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="55" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="55" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="55" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="55" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="55" customWidth="1"/>
+    <col min="12" max="12" width="17" style="55" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="55" customWidth="1"/>
+    <col min="14" max="16384" width="22.28515625" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:21" s="52" customFormat="1">
+      <c r="A1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="52" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:21" s="53" customFormat="1">
+      <c r="A2" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="38" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="56">
         <f t="shared" ref="E2:E3" ca="1" si="0">TODAY()</f>
-        <v>44578</v>
-      </c>
-      <c r="F2" s="46" t="s">
+        <v>44657</v>
+      </c>
+      <c r="F2" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="47">
+      <c r="G2" s="62">
         <v>1371544234</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="I2" s="49">
+      <c r="I2" s="64">
         <v>1771709147</v>
       </c>
-      <c r="J2" s="49">
+      <c r="J2" s="64">
         <v>1771709147</v>
       </c>
-      <c r="K2" s="45">
+      <c r="K2" s="60">
         <v>223.3</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="M2" s="36" t="s">
+      <c r="M2" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="34">
+      <c r="E3" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>44578</v>
-      </c>
-      <c r="F3" s="54" t="s">
+        <v>44657</v>
+      </c>
+      <c r="F3" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="G3" s="55">
+      <c r="G3" s="49">
         <v>3195635219</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="55">
         <v>608519016</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="54" t="s">
         <v>164</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="58" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:21">
+      <c r="A4" s="55" t="s">
         <v>147</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="55">
         <v>2058887593</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
+    <row r="5" spans="1:21">
+      <c r="A5" s="66" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="55">
         <v>2058887593</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:21">
+      <c r="A6" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="F6" s="54" t="s">
+      <c r="F6" s="65" t="s">
         <v>152</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="69">
         <v>1580543906</v>
       </c>
-      <c r="L6" s="35" t="s">
+      <c r="L6" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="M6" s="58" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+    <row r="7" spans="1:21">
+      <c r="A7" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="65" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="69">
         <v>1580543906</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+    <row r="8" spans="1:21">
+      <c r="A8" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="65" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" s="69">
+        <v>2058887593</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" s="70">
+        <v>5456788407</v>
+      </c>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="51"/>
+      <c r="U9" s="51"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="G10" s="70">
+        <v>5456788407</v>
+      </c>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="51"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="G11" s="70">
+        <v>5456788407</v>
+      </c>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="51"/>
+      <c r="U11" s="51"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="51"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="51"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="55" t="s">
+        <v>187</v>
+      </c>
+      <c r="F13" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="G13" s="70">
+        <v>5456788407</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2051,56 +2572,56 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="69">
+      <c r="C2" s="36">
         <v>44387</v>
       </c>
-      <c r="D2" s="69">
+      <c r="D2" s="36">
         <v>44207</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="10" t="s">
         <v>135</v>
       </c>
       <c r="F2">
@@ -2113,21 +2634,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>153</v>
       </c>
       <c r="B3" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="69">
+      <c r="C3" s="36">
         <v>44387</v>
       </c>
-      <c r="D3" s="69">
+      <c r="D3" s="36">
         <v>44207</v>
       </c>
-      <c r="E3" s="20" t="s">
-        <v>135</v>
+      <c r="E3" s="10" t="s">
+        <v>186</v>
       </c>
       <c r="F3">
         <v>15</v>
@@ -2146,30 +2667,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59830DF0-FAD5-472D-8467-4240A14AC5A6}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="73" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>153</v>
       </c>
@@ -2178,6 +2703,20 @@
       </c>
       <c r="C2" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="72">
+        <v>50</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="75">
+        <v>44565</v>
       </c>
     </row>
   </sheetData>
@@ -2186,6 +2725,61 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA7C2A6-2F8A-4DE2-A755-BF21B3B31F5B}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="77" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="80" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="77" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="79" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="81">
+        <v>5456788407</v>
+      </c>
+      <c r="E2" s="76" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3520C8-D792-4977-99E0-C45876A8E20A}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -2193,142 +2787,142 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" s="5" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:10">
+      <c r="A2" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="29" t="str">
+      <c r="B2" s="18" t="str">
         <f>searchValues!F3</f>
         <v>GZQtMQMuM Automation</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="17">
         <f>searchValues!G3</f>
         <v>3195635219</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:10">
+      <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2337,330 +2931,151 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B240F2F-8AD3-49E3-9150-9222387F22C2}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="43" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="43" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="43" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="43"/>
+    <col min="1" max="1" width="22.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="27" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="27" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:9" s="23" customFormat="1">
+      <c r="A1" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="90" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="H1" s="99" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1" s="99" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="41" t="str">
+      <c r="B2" s="25" t="str">
         <f>searchValues!I3</f>
         <v>0266579499</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="87">
         <v>1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="B3" s="87"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="B4" s="87"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="B5" s="87"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03A182C-4A83-40EC-82BA-4154075170BB}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="26"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>130</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6705243-A037-4CA9-B29E-68E745D48062}">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="7" t="str">
-        <f>searchValues!F3</f>
-        <v>GZQtMQMuM Automation</v>
-      </c>
-      <c r="C2" s="7" t="str">
-        <f>searchValues!F3</f>
-        <v>GZQtMQMuM Automation</v>
-      </c>
-      <c r="D2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-    </row>
-    <row r="7" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
-        <v>147</v>
-      </c>
-      <c r="B7" s="8" t="str">
-        <f>searchValues!$F$5</f>
-        <v>Nick Automation</v>
-      </c>
-      <c r="C7" s="8" t="str">
-        <f>searchValues!$F$5</f>
-        <v>Nick Automation</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="67">
-        <v>3499</v>
-      </c>
-      <c r="H7" s="67">
-        <v>3499</v>
-      </c>
-      <c r="I7" s="63">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="66" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="8" t="str">
-        <f>searchValues!$F$5</f>
-        <v>Nick Automation</v>
-      </c>
-      <c r="C8" s="8" t="str">
-        <f>searchValues!$F$5</f>
-        <v>Nick Automation</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="67">
-        <v>3499</v>
-      </c>
-      <c r="H8" s="67">
-        <v>3499</v>
-      </c>
-      <c r="I8" s="63">
-        <v>100</v>
+      <c r="B6" s="87"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87" t="s">
+        <v>190</v>
+      </c>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87" t="s">
+        <v>191</v>
+      </c>
+      <c r="I7" s="100">
+        <v>44716</v>
       </c>
     </row>
   </sheetData>
@@ -2670,112 +3085,320 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6623F5E3-B6AD-4B62-877A-4DCEFEC224B3}">
-  <dimension ref="A1:K3"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03A182C-4A83-40EC-82BA-4154075170BB}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="37.5703125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="31" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2">
-        <f>searchValues!$G$5</f>
-        <v>2058887593</v>
-      </c>
-      <c r="C2" t="str">
-        <f>searchValues!$F$4</f>
-        <v>Nick Automation</v>
-      </c>
-      <c r="D2" s="64" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="64">
-        <v>100</v>
-      </c>
-      <c r="F2" s="65">
-        <f ca="1">TODAY()</f>
-        <v>44578</v>
-      </c>
-      <c r="G2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3">
-        <f>searchValues!$G$5</f>
-        <v>2058887593</v>
-      </c>
-      <c r="C3" t="str">
-        <f>searchValues!$F$4</f>
-        <v>Nick Automation</v>
-      </c>
-      <c r="F3" s="65">
-        <f ca="1">TODAY()</f>
-        <v>44578</v>
-      </c>
-      <c r="H3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I3" t="s">
-        <v>146</v>
+      <c r="B1" s="30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="83" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="71">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6705243-A037-4CA9-B29E-68E745D48062}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" style="93" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.85546875" style="93" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="93" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="93" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="93" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="93" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="93" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="93" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="93"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="91" customFormat="1">
+      <c r="A1" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="90" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="90" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="90" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="90" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="90" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="91" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="86" t="str">
+        <f>searchValues!F3</f>
+        <v>GZQtMQMuM Automation</v>
+      </c>
+      <c r="C2" s="86" t="str">
+        <f>searchValues!F3</f>
+        <v>GZQtMQMuM Automation</v>
+      </c>
+      <c r="D2" s="85" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="89" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="87"/>
+      <c r="H2" s="89" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="87" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="87" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="92" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="93" t="str">
+        <f>searchValues!$F$5</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="C7" s="93" t="str">
+        <f>searchValues!$F$5</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="E7" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="94">
+        <v>3499</v>
+      </c>
+      <c r="H7" s="94">
+        <v>3499</v>
+      </c>
+      <c r="I7" s="94">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="95" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="93" t="str">
+        <f>searchValues!$F$5</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="C8" s="93" t="str">
+        <f>searchValues!$F$5</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="E8" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="94">
+        <v>3499</v>
+      </c>
+      <c r="H8" s="94">
+        <v>3499</v>
+      </c>
+      <c r="I8" s="94">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="87" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="93" t="str">
+        <f>searchValues!$F$5</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="C9" s="93" t="str">
+        <f>searchValues!$F$5</f>
+        <v>Nick Automation</v>
+      </c>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="88"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="94"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="85"/>
+      <c r="E10" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="92" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="85"/>
+      <c r="E11" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" s="85"/>
+      <c r="E12" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="85"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="93" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="85"/>
+      <c r="E13" s="67" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commissions feature - tests added
</commit_message>
<xml_diff>
--- a/testdata/BillingCenter.xlsx
+++ b/testdata/BillingCenter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIG\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CIG\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D50062-C8C5-418A-9F2E-985CF586C6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62AD4EB-3B96-4A6E-9021-87DFBD5AFE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="9" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,13 @@
     <sheet name="Policy" sheetId="3" r:id="rId7"/>
     <sheet name="DirectBillPayment" sheetId="11" r:id="rId8"/>
     <sheet name="AcctSummary" sheetId="5" r:id="rId9"/>
-    <sheet name="Disbursement" sheetId="12" r:id="rId10"/>
-    <sheet name="AcctDetails" sheetId="6" r:id="rId11"/>
-    <sheet name="Contacts" sheetId="7" r:id="rId12"/>
-    <sheet name="Invoices" sheetId="4" r:id="rId13"/>
-    <sheet name="PolicySummary" sheetId="8" r:id="rId14"/>
-    <sheet name="PolicyDetails" sheetId="9" r:id="rId15"/>
+    <sheet name="Documents" sheetId="17" r:id="rId10"/>
+    <sheet name="Disbursement" sheetId="12" r:id="rId11"/>
+    <sheet name="AcctDetails" sheetId="6" r:id="rId12"/>
+    <sheet name="Contacts" sheetId="7" r:id="rId13"/>
+    <sheet name="Invoices" sheetId="4" r:id="rId14"/>
+    <sheet name="PolicySummary" sheetId="8" r:id="rId15"/>
+    <sheet name="PolicyDetails" sheetId="9" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,9 +38,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="194">
   <si>
     <t>su</t>
   </si>
@@ -99,27 +98,6 @@
   </si>
   <si>
     <t>tallen</t>
-  </si>
-  <si>
-    <t>User1</t>
-  </si>
-  <si>
-    <t>User2</t>
-  </si>
-  <si>
-    <t>User3</t>
-  </si>
-  <si>
-    <t>User4</t>
-  </si>
-  <si>
-    <t>User5</t>
-  </si>
-  <si>
-    <t>User6</t>
-  </si>
-  <si>
-    <t>User7</t>
   </si>
   <si>
     <t>TD_AccountName</t>
@@ -626,6 +604,33 @@
   </si>
   <si>
     <t>Payment Declined</t>
+  </si>
+  <si>
+    <t>UploadDocuments</t>
+  </si>
+  <si>
+    <t>FileType</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>DocumentType</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>DocumentsName</t>
+  </si>
+  <si>
+    <t>Sample_CSV</t>
+  </si>
+  <si>
+    <t>Commissions</t>
   </si>
 </sst>
 </file>
@@ -639,7 +644,7 @@
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="167" formatCode="dd\/mm\/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,6 +688,13 @@
     </font>
     <font>
       <sz val="9.8000000000000007"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -756,7 +768,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -790,11 +802,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -873,31 +898,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1030,6 +1036,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1310,318 +1320,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="54.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="41" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="41"/>
+    <col min="1" max="1" width="10.1796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="43" customFormat="1">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:6" s="40" customFormat="1">
+      <c r="A1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>62</v>
+      <c r="B1" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="38" t="s">
         <v>1</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="B3" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>5</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="B4" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="38" t="s">
         <v>7</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="B5" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>9</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="B6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="38" t="s">
         <v>11</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="B7" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="38" t="s">
         <v>13</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="B8" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="38" t="s">
         <v>15</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="B9" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="38" t="s">
         <v>1</v>
       </c>
+      <c r="D9" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="40" t="s">
+      <c r="A10" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="45" t="s">
-        <v>147</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="B12" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="B16" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="41" t="s">
-        <v>153</v>
-      </c>
-      <c r="B17" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="85" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="85" t="s">
-        <v>63</v>
+      <c r="D10" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AC001A-74A5-4FAE-8749-8B1BC776DB6F}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" customWidth="1"/>
+    <col min="5" max="5" width="22.90625" customWidth="1"/>
+    <col min="6" max="6" width="26.453125" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" customWidth="1"/>
+    <col min="8" max="8" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="75" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="90" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6623F5E3-B6AD-4B62-877A-4DCEFEC224B3}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -1629,15 +1625,15 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1645,35 +1641,35 @@
         <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>144</v>
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="33" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B2">
         <f>searchValues!$G$5</f>
@@ -1684,28 +1680,28 @@
         <v>Nick Automation</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E2" s="34">
         <v>100</v>
       </c>
       <c r="F2" s="35">
         <f ca="1">TODAY()</f>
-        <v>44657</v>
+        <v>44663</v>
       </c>
       <c r="G2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="H2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="I2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B3">
         <f>searchValues!$G$5</f>
@@ -1717,18 +1713,18 @@
       </c>
       <c r="F3" s="35">
         <f ca="1">TODAY()</f>
-        <v>44657</v>
+        <v>44663</v>
       </c>
       <c r="H3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="I3" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B4">
         <f>searchValues!$G$5</f>
@@ -1739,22 +1735,22 @@
         <v>Nick Automation</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E4">
         <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="H4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="I4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1762,7 +1758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C58BF8B-1280-4F12-9EAD-0C522762E5C1}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1770,20 +1766,20 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="14"/>
+    <col min="7" max="7" width="20.453125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="9" customFormat="1">
@@ -1791,39 +1787,39 @@
         <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>76</v>
-      </c>
       <c r="J1" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="20" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" s="21" t="str">
         <f>searchValues!F3</f>
@@ -1834,27 +1830,27 @@
         <v>3195635219</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E2" s="28">
         <f ca="1">searchValues!E3</f>
-        <v>44657</v>
+        <v>44663</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="18" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1863,7 +1859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BA4B8D-994F-445A-8329-A78DC1606E04}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1871,14 +1867,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1886,40 +1882,40 @@
         <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="75">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="58">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C2" t="str">
         <f>searchValues!F3</f>
         <v>GZQtMQMuM Automation</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G2" t="str">
         <f>searchValues!M3</f>
@@ -1928,19 +1924,19 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G3">
         <f>searchValues!M4</f>
@@ -1952,7 +1948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729A753F-FC84-49D2-8EB2-5A2921F6B535}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1960,17 +1956,17 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1978,58 +1974,58 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C2" s="29">
         <f ca="1">searchValues!E3</f>
-        <v>44657</v>
+        <v>44663</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" t="s">
         <v>90</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2042,24 +2038,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71F8AC9-A36C-49D9-9891-077F11566646}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2067,75 +2063,98 @@
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="98" t="s">
-        <v>184</v>
-      </c>
-      <c r="I1" s="98"/>
+        <v>34</v>
+      </c>
+      <c r="H1" s="91" t="s">
+        <v>177</v>
+      </c>
+      <c r="I1" s="91"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="97" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="96" t="s">
-        <v>181</v>
-      </c>
-      <c r="C3" s="96" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="96" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="96" t="s">
-        <v>182</v>
-      </c>
-      <c r="F3" s="96" t="s">
-        <v>102</v>
-      </c>
-      <c r="G3" s="96" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="96" t="s">
-        <v>183</v>
+      <c r="A3" s="90" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="89" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="89" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="89" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="89" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="89" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" s="89" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="89" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" s="89" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="89" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2144,22 +2163,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222CFAE0-9168-4C02-A943-4F9BE574003A}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2167,58 +2188,84 @@
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" t="str">
         <f>searchValues!J3</f>
         <v>0266579499-1</v>
       </c>
       <c r="C2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
         <v>94</v>
       </c>
-      <c r="D2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="89" t="s">
         <v>101</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E3" s="89" t="s">
         <v>94</v>
       </c>
-      <c r="G2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" t="s">
-        <v>57</v>
+      <c r="F3" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="89" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="89" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="89" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2229,337 +2276,353 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609C42BF-E54F-4C6E-8490-1C1A1918364C}">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:G13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="22.26953125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="47.140625" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="55" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="55" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="55" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" style="55" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="55" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="55" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="55" customWidth="1"/>
-    <col min="12" max="12" width="17" style="55" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="55" customWidth="1"/>
-    <col min="14" max="16384" width="22.28515625" style="55"/>
+    <col min="1" max="1" width="47.1796875" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" style="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" style="48" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" style="48" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7265625" style="48" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" style="48" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7265625" style="48" customWidth="1"/>
+    <col min="11" max="11" width="12.54296875" style="48" customWidth="1"/>
+    <col min="12" max="12" width="17" style="48" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" style="48" customWidth="1"/>
+    <col min="14" max="16384" width="22.26953125" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="52" customFormat="1">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:21" s="45" customFormat="1">
+      <c r="A1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="J1" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="L1" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="M1" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="52" t="s">
+    </row>
+    <row r="2" spans="1:21" s="46" customFormat="1">
+      <c r="A2" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="B2" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="48"/>
+      <c r="D2" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="49">
+        <f t="shared" ref="E2:E3" ca="1" si="0">TODAY()</f>
+        <v>44663</v>
+      </c>
+      <c r="F2" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="G2" s="55">
+        <v>1371544234</v>
+      </c>
+      <c r="H2" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="57">
+        <v>1771709147</v>
+      </c>
+      <c r="J2" s="57">
+        <v>1771709147</v>
+      </c>
+      <c r="K2" s="53">
+        <v>223.3</v>
+      </c>
+      <c r="L2" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="J1" s="52" t="s">
-        <v>129</v>
-      </c>
-      <c r="K1" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="L1" s="52" t="s">
-        <v>121</v>
-      </c>
-      <c r="M1" s="52" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" s="53" customFormat="1">
-      <c r="A2" s="55" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="60" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="56">
-        <f t="shared" ref="E2:E3" ca="1" si="0">TODAY()</f>
-        <v>44657</v>
-      </c>
-      <c r="F2" s="61" t="s">
-        <v>124</v>
-      </c>
-      <c r="G2" s="62">
-        <v>1371544234</v>
-      </c>
-      <c r="H2" s="63" t="s">
-        <v>128</v>
-      </c>
-      <c r="I2" s="64">
-        <v>1771709147</v>
-      </c>
-      <c r="J2" s="64">
-        <v>1771709147</v>
-      </c>
-      <c r="K2" s="60">
-        <v>223.3</v>
-      </c>
-      <c r="L2" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="M2" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
+      <c r="M2" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="56">
+      <c r="A3" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>44657</v>
-      </c>
-      <c r="F3" s="65" t="s">
+        <v>44663</v>
+      </c>
+      <c r="F3" s="58" t="s">
+        <v>159</v>
+      </c>
+      <c r="G3" s="42">
+        <v>3195635219</v>
+      </c>
+      <c r="H3" s="48">
+        <v>608519016</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="L3" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="M3" s="51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" s="48">
+        <v>2058887593</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="59" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="48">
+        <v>2058887593</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" s="62">
+        <v>1580543906</v>
+      </c>
+      <c r="L6" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="M6" s="51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="58" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7" s="62">
+        <v>1580543906</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" s="62">
+        <v>2058887593</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="G3" s="49">
-        <v>3195635219</v>
-      </c>
-      <c r="H3" s="55">
-        <v>608519016</v>
-      </c>
-      <c r="I3" s="54" t="s">
+      <c r="G9" s="63">
+        <v>5456788407</v>
+      </c>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="44"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="44"/>
+      <c r="U9" s="44"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="63">
+        <v>5456788407</v>
+      </c>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="44"/>
+      <c r="T10" s="44"/>
+      <c r="U10" s="44"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" s="63">
+        <v>5456788407</v>
+      </c>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="44"/>
+      <c r="U11" s="44"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="J3" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="L3" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="M3" s="58" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="55" t="s">
-        <v>147</v>
-      </c>
-      <c r="F4" s="55" t="s">
-        <v>149</v>
-      </c>
-      <c r="G4" s="55">
-        <v>2058887593</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="66" t="s">
-        <v>148</v>
-      </c>
-      <c r="F5" s="55" t="s">
-        <v>149</v>
-      </c>
-      <c r="G5" s="55">
-        <v>2058887593</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="53" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="67" t="s">
-        <v>151</v>
-      </c>
-      <c r="F6" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="G6" s="69">
-        <v>1580543906</v>
-      </c>
-      <c r="L6" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="M6" s="58" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="53" t="s">
-        <v>153</v>
-      </c>
-      <c r="F7" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="G7" s="69">
-        <v>1580543906</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="53" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="61" t="s">
         <v>167</v>
       </c>
-      <c r="F8" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="G8" s="69">
-        <v>2058887593</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="G9" s="70">
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="44"/>
+      <c r="S12" s="44"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="44"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="F13" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="G13" s="63">
         <v>5456788407</v>
       </c>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="51"/>
-      <c r="S9" s="51"/>
-      <c r="T9" s="51"/>
-      <c r="U9" s="51"/>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="G10" s="70">
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="94" t="s">
+        <v>185</v>
+      </c>
+      <c r="F14" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="G14" s="63">
         <v>5456788407</v>
       </c>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="51"/>
-      <c r="Q10" s="51"/>
-      <c r="R10" s="51"/>
-      <c r="S10" s="51"/>
-      <c r="T10" s="51"/>
-      <c r="U10" s="51"/>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="G11" s="70">
-        <v>5456788407</v>
-      </c>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="51"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="51"/>
-      <c r="S11" s="51"/>
-      <c r="T11" s="51"/>
-      <c r="U11" s="51"/>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="68" t="s">
-        <v>174</v>
-      </c>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="51"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="51"/>
-      <c r="T12" s="51"/>
-      <c r="U12" s="51"/>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="55" t="s">
-        <v>187</v>
-      </c>
-      <c r="F13" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="G13" s="70">
-        <v>5456788407</v>
-      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="90"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2569,16 +2632,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1624AA-EFC2-4B9A-B805-8486152D6359}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2587,33 +2651,33 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C2" s="36">
         <v>44387</v>
@@ -2622,7 +2686,7 @@
         <v>44207</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>135</v>
+        <v>179</v>
       </c>
       <c r="F2">
         <v>15</v>
@@ -2636,10 +2700,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C3" s="36">
         <v>44387</v>
@@ -2648,7 +2712,7 @@
         <v>44207</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F3">
         <v>15</v>
@@ -2659,6 +2723,15 @@
       <c r="H3">
         <v>25</v>
       </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="90"/>
+      <c r="B4" s="95"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2673,11 +2746,11 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2685,37 +2758,37 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D1" s="73" t="s">
-        <v>139</v>
+        <v>155</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B2">
         <v>50</v>
       </c>
       <c r="C2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="67" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="74" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="72">
+      <c r="B3" s="65">
         <v>50</v>
       </c>
-      <c r="C3" s="72" t="s">
-        <v>163</v>
-      </c>
-      <c r="D3" s="75">
+      <c r="C3" s="65" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="68">
         <v>44565</v>
       </c>
     </row>
@@ -2732,46 +2805,46 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="77" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>176</v>
-      </c>
-      <c r="D1" s="80" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="77" t="s">
-        <v>177</v>
+      <c r="B1" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="70" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="78" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="76" t="s">
-        <v>178</v>
-      </c>
-      <c r="C2" s="79" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" s="81">
+      <c r="A2" s="71" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="72" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="74">
         <v>5456788407</v>
       </c>
-      <c r="E2" s="76" t="s">
-        <v>180</v>
+      <c r="E2" s="69" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2783,23 +2856,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3520C8-D792-4977-99E0-C45876A8E20A}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="11" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="5" customFormat="1">
@@ -2807,36 +2880,36 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="15" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" s="18" t="str">
         <f>searchValues!F3</f>
@@ -2847,30 +2920,30 @@
         <v>3195635219</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -2884,7 +2957,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -2898,7 +2971,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -2912,7 +2985,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -2939,142 +3012,142 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.1796875" style="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="27" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="27" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="27"/>
+    <col min="6" max="6" width="15.7265625" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" style="27" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" style="27" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="23" customFormat="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="90" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="90" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="90" t="s">
+      <c r="B1" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="90" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="90" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="99" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1" s="99" t="s">
-        <v>189</v>
+      <c r="C1" s="83" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="92" t="s">
+        <v>181</v>
+      </c>
+      <c r="I1" s="92" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="24" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" s="25" t="str">
         <f>searchValues!I3</f>
         <v>0266579499</v>
       </c>
       <c r="C2" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="80">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="80"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="80"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="80"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="88" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="87" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="87" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="87">
-        <v>1000</v>
-      </c>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="87" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="87" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="87"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="87" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="87" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="87"/>
+      <c r="B6" s="80"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87" t="s">
-        <v>190</v>
-      </c>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87" t="s">
-        <v>191</v>
-      </c>
-      <c r="I7" s="100">
+        <v>180</v>
+      </c>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80" t="s">
+        <v>183</v>
+      </c>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80" t="s">
+        <v>184</v>
+      </c>
+      <c r="I7" s="93">
         <v>44716</v>
       </c>
     </row>
@@ -3093,34 +3166,34 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="31" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="37.54296875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" style="31" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="75" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="83" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="84" t="s">
-        <v>130</v>
+      <c r="A2" s="76" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="B3" s="71">
+      <c r="A3" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="64">
         <v>500</v>
       </c>
     </row>
@@ -3131,269 +3204,284 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6705243-A037-4CA9-B29E-68E745D48062}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="93" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24.85546875" style="93" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="93" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="93" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="93" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="93" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="93" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="93" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="93"/>
+    <col min="1" max="1" width="26.1796875" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.81640625" style="86" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" style="86" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" style="86" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" style="86" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="86" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="86"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="91" customFormat="1">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:9" s="84" customFormat="1">
+      <c r="A1" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="90" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="90" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="90" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="90" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="90" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="90" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="90" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="91" t="s">
-        <v>136</v>
+      <c r="B1" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="83" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="83" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="83" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="84" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="87" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="86" t="str">
+      <c r="A2" s="80" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="79" t="str">
         <f>searchValues!F3</f>
         <v>GZQtMQMuM Automation</v>
       </c>
-      <c r="C2" s="86" t="str">
+      <c r="C2" s="79" t="str">
         <f>searchValues!F3</f>
         <v>GZQtMQMuM Automation</v>
       </c>
-      <c r="D2" s="85" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" s="86" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="89" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="89" t="s">
-        <v>57</v>
+      <c r="D2" s="78" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="82" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="80"/>
+      <c r="H2" s="82" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="87" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
+      <c r="A3" s="80" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="87" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
+      <c r="A4" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="87" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
+      <c r="A5" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="87" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
+      <c r="A6" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="92" t="s">
-        <v>147</v>
-      </c>
-      <c r="B7" s="93" t="str">
+      <c r="A7" s="85" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="86" t="str">
         <f>searchValues!$F$5</f>
         <v>Nick Automation</v>
       </c>
-      <c r="C7" s="93" t="str">
+      <c r="C7" s="86" t="str">
         <f>searchValues!$F$5</f>
         <v>Nick Automation</v>
       </c>
-      <c r="E7" s="86" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="94">
+      <c r="E7" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="87">
         <v>3499</v>
       </c>
-      <c r="H7" s="94">
+      <c r="H7" s="87">
         <v>3499</v>
       </c>
-      <c r="I7" s="94">
+      <c r="I7" s="87">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="95" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="93" t="str">
+      <c r="A8" s="88" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="86" t="str">
         <f>searchValues!$F$5</f>
         <v>Nick Automation</v>
       </c>
-      <c r="C8" s="93" t="str">
+      <c r="C8" s="86" t="str">
         <f>searchValues!$F$5</f>
         <v>Nick Automation</v>
       </c>
-      <c r="E8" s="86" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="94">
+      <c r="E8" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="87">
         <v>3499</v>
       </c>
-      <c r="H8" s="94">
+      <c r="H8" s="87">
         <v>3499</v>
       </c>
-      <c r="I8" s="94">
+      <c r="I8" s="87">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="87" t="s">
-        <v>167</v>
-      </c>
-      <c r="B9" s="93" t="str">
+      <c r="A9" s="80" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="86" t="str">
         <f>searchValues!$F$5</f>
         <v>Nick Automation</v>
       </c>
-      <c r="C9" s="93" t="str">
+      <c r="C9" s="86" t="str">
         <f>searchValues!$F$5</f>
         <v>Nick Automation</v>
       </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="88"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="94"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="81"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="87"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="B10" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="C10" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="D10" s="85"/>
-      <c r="E10" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
+      <c r="A10" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="78"/>
+      <c r="E10" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="92" t="s">
-        <v>168</v>
-      </c>
-      <c r="B11" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="C11" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="D11" s="85"/>
-      <c r="E11" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
+      <c r="A11" s="85" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="78"/>
+      <c r="E11" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="B12" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="C12" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="D12" s="85"/>
-      <c r="E12" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="85"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="85"/>
-      <c r="I12" s="85"/>
+      <c r="A12" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="78"/>
+      <c r="E12" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="93" t="s">
-        <v>187</v>
-      </c>
-      <c r="B13" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="C13" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="D13" s="85"/>
-      <c r="E13" s="67" t="s">
-        <v>71</v>
+      <c r="A13" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="D13" s="78"/>
+      <c r="E13" s="60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="90" t="s">
+        <v>185</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="D14" s="78"/>
+      <c r="E14" s="60" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>